<commit_message>
Added Long term loans variable to the dataset
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/WU/Master/3_WS2020:21/R&amp;P - Money, Credit and Finance/02_Research Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajdakovac/Documents/GitHub/rp-mcf/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22362887-C301-3749-9582-1F3A2C593683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94713B2-AFAC-CD4D-B57C-E7A0258786A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="960" windowWidth="27640" windowHeight="16480" xr2:uid="{CC9B95F3-3BB9-1449-8216-D93773899462}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" xr2:uid="{CC9B95F3-3BB9-1449-8216-D93773899462}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
     <t>Q4-2020</t>
   </si>
@@ -272,13 +263,16 @@
   </si>
   <si>
     <t>Shadow rate</t>
+  </si>
+  <si>
+    <t>Long term loans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -623,15 +617,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB8DCE9-B619-404A-B6A3-826AD971B006}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -650,8 +644,11 @@
       <c r="F1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -670,8 +667,11 @@
       <c r="F2">
         <v>2.0447360090000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>17.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -690,8 +690,11 @@
       <c r="F3">
         <v>2.0753298650000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>18.89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -710,8 +713,11 @@
       <c r="F4">
         <v>2.0028966010000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -730,8 +736,11 @@
       <c r="F5">
         <v>2.1122235599999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>18.82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -750,8 +759,11 @@
       <c r="F6">
         <v>1.9800761060000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -770,8 +782,11 @@
       <c r="F7">
         <v>2.3013087959999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -790,8 +805,11 @@
       <c r="F8">
         <v>2.518025309</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>24.37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -810,8 +828,11 @@
       <c r="F9">
         <v>2.8227288349999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>33.630000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -830,8 +851,11 @@
       <c r="F10">
         <v>3.3606117950000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>29.55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -850,8 +874,11 @@
       <c r="F11">
         <v>3.4797052160000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>30.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -870,8 +897,11 @@
       <c r="F12">
         <v>3.7235367730000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>29.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -890,8 +920,11 @@
       <c r="F13">
         <v>3.910530391</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>26.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -910,8 +943,11 @@
       <c r="F14">
         <v>3.7632808739999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>22.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -930,8 +966,11 @@
       <c r="F15">
         <v>3.964531198</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -950,8 +989,11 @@
       <c r="F16">
         <v>4.0122059969999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>-14.82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -970,8 +1012,11 @@
       <c r="F17">
         <v>4.1591700889999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>-18.329999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -990,8 +1035,11 @@
       <c r="F18">
         <v>3.7536965609999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>-21.77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1010,8 +1058,11 @@
       <c r="F19">
         <v>1.6249197740000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>-15.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1030,8 +1081,11 @@
       <c r="F20">
         <v>0.123994956</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>-45.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1050,8 +1104,11 @@
       <c r="F21">
         <v>0.171480824</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>-27.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1070,8 +1127,11 @@
       <c r="F22">
         <v>-0.42021012200000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>-21.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1090,8 +1150,11 @@
       <c r="F23">
         <v>0.19245778699999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>-15.13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1110,8 +1173,11 @@
       <c r="F24">
         <v>0.212222465</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1130,8 +1196,11 @@
       <c r="F25">
         <v>0.39749030400000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1150,8 +1219,11 @@
       <c r="F26">
         <v>0.804366743</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>17.98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1170,8 +1242,11 @@
       <c r="F27">
         <v>0.52188641099999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1190,8 +1265,11 @@
       <c r="F28">
         <v>0.71147068800000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>22.69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1210,8 +1288,11 @@
       <c r="F29">
         <v>1.340296095</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>23.24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1230,8 +1311,11 @@
       <c r="F30">
         <v>0.40539584400000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>7.51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1250,8 +1334,11 @@
       <c r="F31">
         <v>-0.732679941</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>-24.72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1270,8 +1357,11 @@
       <c r="F32">
         <v>-0.21804300200000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>-30.44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1290,8 +1380,11 @@
       <c r="F33">
         <v>-0.67433711399999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>-2.88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1310,8 +1403,11 @@
       <c r="F34">
         <v>-1.0113929079999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>-17.71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1330,8 +1426,11 @@
       <c r="F35">
         <v>-1.0864902000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>-14.32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1350,8 +1449,11 @@
       <c r="F36">
         <v>-0.62494092800000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>-13.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1370,8 +1472,11 @@
       <c r="F37">
         <v>0.51921321099999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>-11.47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1390,8 +1495,11 @@
       <c r="F38">
         <v>-0.40967663100000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>-1.29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -1410,8 +1518,11 @@
       <c r="F39">
         <v>-0.11825192900000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>-3.41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1430,8 +1541,11 @@
       <c r="F40">
         <v>-0.69596967399999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -1450,8 +1564,11 @@
       <c r="F41">
         <v>-0.86085107900000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -1470,8 +1587,11 @@
       <c r="F42">
         <v>-1.3321349769999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1490,8 +1610,11 @@
       <c r="F43">
         <v>-2.2490178630000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>15.78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -1510,8 +1633,11 @@
       <c r="F44">
         <v>-2.596925685</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1530,8 +1656,11 @@
       <c r="F45">
         <v>-2.3401699310000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>36.93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1550,8 +1679,11 @@
       <c r="F46">
         <v>-2.559260053</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>32.26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1570,8 +1702,11 @@
       <c r="F47">
         <v>-2.5615593799999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>31.96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -1590,8 +1725,11 @@
       <c r="F48">
         <v>-3.7627687019999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -1610,8 +1748,11 @@
       <c r="F49">
         <v>-4.335395503</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1630,8 +1771,11 @@
       <c r="F50">
         <v>-4.5695823249999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>27.34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -1650,8 +1794,11 @@
       <c r="F51">
         <v>-4.5237854500000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -1670,8 +1817,11 @@
       <c r="F52">
         <v>-5.3752556550000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -1690,8 +1840,11 @@
       <c r="F53">
         <v>-5.1359423209999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1710,8 +1863,11 @@
       <c r="F54">
         <v>-5.2563992989999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>18.809999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -1730,8 +1886,11 @@
       <c r="F55">
         <v>-4.8251996320000003</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1749,6 +1908,9 @@
       </c>
       <c r="F56">
         <v>-5.1466281929999997</v>
+      </c>
+      <c r="G56">
+        <v>18.32</v>
       </c>
     </row>
   </sheetData>
@@ -1758,15 +1920,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAC09D4-F2E9-0247-8720-B1B0A2564B18}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -1785,8 +1947,11 @@
       <c r="F1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1799,8 +1964,11 @@
       <c r="E2">
         <v>1.874557894736842</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>8.3699999999999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1816,8 +1984,11 @@
       <c r="E3">
         <v>1.8617473684210528</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>-0.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1833,8 +2004,11 @@
       <c r="E4">
         <v>1.7673421052631577</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>19.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1850,8 +2024,11 @@
       <c r="E5">
         <v>1.7483263157894735</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>-12.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1867,8 +2044,11 @@
       <c r="E6">
         <v>1.8120263157894736</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1884,8 +2064,11 @@
       <c r="E7">
         <v>1.8205736842105262</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1901,8 +2084,11 @@
       <c r="E8">
         <v>1.8191578947368421</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1918,8 +2104,11 @@
       <c r="E9">
         <v>1.8127789473684206</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1935,8 +2124,11 @@
       <c r="E10">
         <v>1.8551526315789475</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1952,8 +2144,11 @@
       <c r="E11">
         <v>1.853378947368421</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1969,8 +2164,11 @@
       <c r="E12">
         <v>1.7903999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>23.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1989,8 +2187,11 @@
       <c r="F13">
         <v>-5.1466281929999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>18.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2009,8 +2210,11 @@
       <c r="F14">
         <v>-4.8251996320000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2029,8 +2233,11 @@
       <c r="F15">
         <v>-5.2563992989999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>18.809999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2049,8 +2256,11 @@
       <c r="F16">
         <v>-5.1359423209999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2069,8 +2279,11 @@
       <c r="F17">
         <v>-5.3752556550000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2089,8 +2302,11 @@
       <c r="F18">
         <v>-4.5237854500000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2109,8 +2325,11 @@
       <c r="F19">
         <v>-4.5695823249999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>27.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2129,8 +2348,11 @@
       <c r="F20">
         <v>-4.335395503</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2149,8 +2371,11 @@
       <c r="F21">
         <v>-3.7627687019999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2169,8 +2394,11 @@
       <c r="F22">
         <v>-2.5615593799999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>31.96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2189,8 +2417,11 @@
       <c r="F23">
         <v>-2.559260053</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>32.26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2209,8 +2440,11 @@
       <c r="F24">
         <v>-2.3401699310000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>36.93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2229,8 +2463,11 @@
       <c r="F25">
         <v>-2.596925685</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2249,8 +2486,11 @@
       <c r="F26">
         <v>-2.2490178630000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>15.78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2269,8 +2509,11 @@
       <c r="F27">
         <v>-1.3321349769999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2289,8 +2532,11 @@
       <c r="F28">
         <v>-0.86085107900000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2309,8 +2555,11 @@
       <c r="F29">
         <v>-0.69596967399999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2329,8 +2578,11 @@
       <c r="F30">
         <v>-0.11825192900000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>-3.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2349,8 +2601,11 @@
       <c r="F31">
         <v>-0.40967663100000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>-1.29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2369,8 +2624,11 @@
       <c r="F32">
         <v>0.51921321099999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>-11.47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2389,8 +2647,11 @@
       <c r="F33">
         <v>-0.62494092800000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>-13.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2409,8 +2670,11 @@
       <c r="F34">
         <v>-1.0864902000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>-14.32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2429,8 +2693,11 @@
       <c r="F35">
         <v>-1.0113929079999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>-17.71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2449,8 +2716,11 @@
       <c r="F36">
         <v>-0.67433711399999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>-2.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2469,8 +2739,11 @@
       <c r="F37">
         <v>-0.21804300200000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>-30.44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2489,8 +2762,11 @@
       <c r="F38">
         <v>-0.732679941</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>-24.72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2509,8 +2785,11 @@
       <c r="F39">
         <v>0.40539584400000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>7.51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2529,8 +2808,11 @@
       <c r="F40">
         <v>1.340296095</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>23.24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2549,8 +2831,11 @@
       <c r="F41">
         <v>0.71147068800000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>22.69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2569,8 +2854,11 @@
       <c r="F42">
         <v>0.52188641099999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2589,8 +2877,11 @@
       <c r="F43">
         <v>0.804366743</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>17.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2609,8 +2900,11 @@
       <c r="F44">
         <v>0.39749030400000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2629,8 +2923,11 @@
       <c r="F45">
         <v>0.212222465</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2649,8 +2946,11 @@
       <c r="F46">
         <v>0.19245778699999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>-15.13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2669,8 +2969,11 @@
       <c r="F47">
         <v>-0.42021012200000002</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>-21.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2689,8 +2992,11 @@
       <c r="F48">
         <v>0.171480824</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>-27.57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2709,8 +3015,11 @@
       <c r="F49">
         <v>0.123994956</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>-45.95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2729,8 +3038,11 @@
       <c r="F50">
         <v>1.6249197740000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>-15.34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2749,8 +3061,11 @@
       <c r="F51">
         <v>3.7536965609999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>-21.77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2769,8 +3084,11 @@
       <c r="F52">
         <v>4.1591700889999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>-18.329999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2789,8 +3107,11 @@
       <c r="F53">
         <v>4.0122059969999997</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>-14.82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2809,8 +3130,11 @@
       <c r="F54">
         <v>3.964531198</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2829,8 +3153,11 @@
       <c r="F55">
         <v>3.7632808739999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>22.78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2849,8 +3176,11 @@
       <c r="F56">
         <v>3.910530391</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>26.41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2869,8 +3199,11 @@
       <c r="F57">
         <v>3.7235367730000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>29.62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2889,8 +3222,11 @@
       <c r="F58">
         <v>3.4797052160000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>30.32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2909,8 +3245,11 @@
       <c r="F59">
         <v>3.3606117950000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>29.55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2929,8 +3268,11 @@
       <c r="F60">
         <v>2.8227288349999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>33.630000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2949,8 +3291,11 @@
       <c r="F61">
         <v>2.518025309</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>24.37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2969,8 +3314,11 @@
       <c r="F62">
         <v>2.3013087959999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2989,8 +3337,11 @@
       <c r="F63">
         <v>1.9800761060000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3009,8 +3360,11 @@
       <c r="F64">
         <v>2.1122235599999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>18.82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -3029,8 +3383,11 @@
       <c r="F65">
         <v>2.0028966010000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3049,8 +3406,11 @@
       <c r="F66">
         <v>2.0753298650000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>18.89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3069,8 +3429,11 @@
       <c r="F67">
         <v>2.0447360090000002</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>17.82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3086,8 +3449,11 @@
       <c r="E68">
         <v>1.7594615384615382</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>21.94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3103,8 +3469,11 @@
       <c r="E69">
         <v>1.7685615384615383</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>31.54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3120,8 +3489,11 @@
       <c r="E70">
         <v>1.7196499999999997</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3137,8 +3509,11 @@
       <c r="E71">
         <v>1.7326416666666669</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3154,8 +3529,11 @@
       <c r="E72">
         <v>1.6825500000000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>-17.079999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3170,6 +3548,9 @@
       </c>
       <c r="E73">
         <v>1.6802499999999998</v>
+      </c>
+      <c r="G73">
+        <v>-1.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>